<commit_message>
STU_MTCUXR: Llenado de la matriz
</commit_message>
<xml_diff>
--- a/STU/Analisis y Diseño/STU_MTCUXR.xlsx
+++ b/STU/Analisis y Diseño/STU_MTCUXR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jramirezh2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\workspace\projects\RPJA\STU\Analisis y Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>CUS01: Busqueda de vehiculos</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>RQ10: Compartir en redes sociales</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,11 +183,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +475,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,71 +490,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="Q2" s="2"/>
@@ -558,141 +564,153 @@
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="B3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>